<commit_message>
Fix in total percent formulas on Info sheet
</commit_message>
<xml_diff>
--- a/Modry_Zivot.xlsx
+++ b/Modry_Zivot.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/76781d05666600c8/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.benedeki\Programming\Shared\ModryZivot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1482" documentId="11_AFAD60F5616DA92C5213941510834FE6741F2CD2" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D031B01D-377A-44DB-8FCB-1F03838573A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80369E4A-BE45-4273-BDFE-3CD653723FE0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="315" windowWidth="25950" windowHeight="19650" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23325" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="6" r:id="rId1"/>
@@ -493,7 +493,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="[$]dd/mm/yyyy;@" x16r2:formatCode16="[$-en-001,1]dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$]dd/mm/yyyy;@" x16r2:formatCode16="[$-en-001,1]dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -856,7 +856,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -888,7 +888,144 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="93">
+  <dxfs count="47">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -914,6 +1051,76 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1265,720 +1472,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2275,7 +1768,7 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>January 
@@ -2416,7 +1909,7 @@
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
-        <v>https://d.docs.live.net/76781d05666600c8/Documents/[Modry_Zivot.xlsx]1</v>
+        <v>C:\Users\david.benedeki\Programming\Shared\ModryZivot\[Modry_Zivot.xlsx]1</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -2491,35 +1984,35 @@
         <v>Total %</v>
       </c>
       <c r="M4" s="23">
-        <f ca="1">IFERROR(M$2/$AA4*100, "")</f>
+        <f t="shared" ref="M4:T4" ca="1" si="2">IFERROR(M$2/$AA4*100, "")</f>
         <v>0</v>
       </c>
       <c r="N4" s="23">
-        <f ca="1">IFERROR(N$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="O4" s="23">
-        <f ca="1">IFERROR(O$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="23">
-        <f ca="1">IFERROR(P$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="Q4" s="23">
-        <f ca="1">IFERROR(Q$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="R4" s="23">
-        <f ca="1">IFERROR(R$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="S4" s="23">
-        <f ca="1">IFERROR(S$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="T4" s="24">
-        <f ca="1">IFERROR(T$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AA4" s="6">
@@ -2926,7 +2419,7 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="A30:A32">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2973,7 +2466,7 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>October 
@@ -3114,7 +2607,7 @@
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
-        <v>https://d.docs.live.net/76781d05666600c8/Documents/[Modry_Zivot.xlsx]10</v>
+        <v>C:\Users\david.benedeki\Programming\Shared\ModryZivot\[Modry_Zivot.xlsx]10</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -3189,35 +2682,35 @@
         <v>Total %</v>
       </c>
       <c r="M4" s="23">
-        <f ca="1">IFERROR(M$2/$AA4*100, "")</f>
+        <f t="shared" ref="M4:T4" ca="1" si="2">IFERROR(M$2/$AA4*100, "")</f>
         <v>0</v>
       </c>
       <c r="N4" s="23">
-        <f ca="1">IFERROR(N$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="O4" s="23">
-        <f ca="1">IFERROR(O$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="23">
-        <f ca="1">IFERROR(P$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="Q4" s="23">
-        <f ca="1">IFERROR(Q$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="R4" s="23">
-        <f ca="1">IFERROR(R$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="S4" s="23">
-        <f ca="1">IFERROR(S$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="T4" s="24">
-        <f ca="1">IFERROR(T$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AA4" s="6">
@@ -3624,18 +3117,18 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="A30:A32">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:I32">
-    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="2" stopIfTrue="1">
       <formula>$A2=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3671,7 +3164,7 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>November 
@@ -3812,7 +3305,7 @@
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
-        <v>https://d.docs.live.net/76781d05666600c8/Documents/[Modry_Zivot.xlsx]11</v>
+        <v>C:\Users\david.benedeki\Programming\Shared\ModryZivot\[Modry_Zivot.xlsx]11</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -3887,35 +3380,35 @@
         <v>Total %</v>
       </c>
       <c r="M4" s="23">
-        <f ca="1">IFERROR(M$2/$AA4*100, "")</f>
+        <f t="shared" ref="M4:T4" ca="1" si="2">IFERROR(M$2/$AA4*100, "")</f>
         <v>0</v>
       </c>
       <c r="N4" s="23">
-        <f ca="1">IFERROR(N$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="O4" s="23">
-        <f ca="1">IFERROR(O$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="23">
-        <f ca="1">IFERROR(P$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="Q4" s="23">
-        <f ca="1">IFERROR(Q$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="R4" s="23">
-        <f ca="1">IFERROR(R$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="S4" s="23">
-        <f ca="1">IFERROR(S$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="T4" s="24">
-        <f ca="1">IFERROR(T$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AA4" s="6">
@@ -4322,18 +3815,18 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="A30:A32">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:I32">
-    <cfRule type="expression" dxfId="8" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>$A2=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4369,7 +3862,7 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>December 
@@ -4510,7 +4003,7 @@
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
-        <v>https://d.docs.live.net/76781d05666600c8/Documents/[Modry_Zivot.xlsx]12</v>
+        <v>C:\Users\david.benedeki\Programming\Shared\ModryZivot\[Modry_Zivot.xlsx]12</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -4585,35 +4078,35 @@
         <v>Total %</v>
       </c>
       <c r="M4" s="23">
-        <f ca="1">IFERROR(M$2/$AA4*100, "")</f>
+        <f t="shared" ref="M4:T4" ca="1" si="2">IFERROR(M$2/$AA4*100, "")</f>
         <v>0</v>
       </c>
       <c r="N4" s="23">
-        <f ca="1">IFERROR(N$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="O4" s="23">
-        <f ca="1">IFERROR(O$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="23">
-        <f ca="1">IFERROR(P$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="Q4" s="23">
-        <f ca="1">IFERROR(Q$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="R4" s="23">
-        <f ca="1">IFERROR(R$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="S4" s="23">
-        <f ca="1">IFERROR(S$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="T4" s="24">
-        <f ca="1">IFERROR(T$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AA4" s="6">
@@ -5020,18 +4513,18 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="A30:A32">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:I32">
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>$A2=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5050,7 +4543,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5067,7 +4560,7 @@
     <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="87.75" x14ac:dyDescent="0.25">
       <c r="F1" s="25" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
         <v>Teeth brushing</v>
@@ -5163,7 +4656,7 @@
       </c>
       <c r="P2" s="48">
         <f ca="1">'1'!X2+'2'!X2+'3'!X2+'4'!X2+'5'!X2+'6'!X2+'7'!X2+'8'!X2+'9'!X2+'10'!X2+'11'!X2+'12'!X2</f>
-        <v>249.69687268518464</v>
+        <v>260.72448657407222</v>
       </c>
       <c r="Q2" s="49">
         <f ca="1">'1'!AA4+'2'!AA4+'3'!AA4+'4'!AA4+'5'!AA4+'6'!AA4+'7'!AA4+'8'!AA4+'9'!AA4+'10'!AA4+'11'!AA4+'12'!AA4</f>
@@ -5187,7 +4680,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="43">
-        <f t="shared" ref="G3:N3" ca="1" si="0">100*G$2/$P2</f>
+        <f t="shared" ref="G3:M3" ca="1" si="0">100*G$2/$P2</f>
         <v>0</v>
       </c>
       <c r="H3" s="43">
@@ -5215,7 +4708,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="44">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">100*N$2/8/$P2</f>
         <v>0</v>
       </c>
     </row>
@@ -5265,7 +4758,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="47">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">100*N$2/8/$Q2</f>
         <v>0</v>
       </c>
     </row>
@@ -5804,7 +5297,7 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>Ferbuary 
@@ -5945,7 +5438,7 @@
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
-        <v>https://d.docs.live.net/76781d05666600c8/Documents/[Modry_Zivot.xlsx]2</v>
+        <v>C:\Users\david.benedeki\Programming\Shared\ModryZivot\[Modry_Zivot.xlsx]2</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -6020,35 +5513,35 @@
         <v>Total %</v>
       </c>
       <c r="M4" s="23">
-        <f ca="1">IFERROR(M$2/$AA4*100, "")</f>
+        <f t="shared" ref="M4:T4" ca="1" si="2">IFERROR(M$2/$AA4*100, "")</f>
         <v>0</v>
       </c>
       <c r="N4" s="23">
-        <f ca="1">IFERROR(N$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="O4" s="23">
-        <f ca="1">IFERROR(O$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="23">
-        <f ca="1">IFERROR(P$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="Q4" s="23">
-        <f ca="1">IFERROR(Q$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="R4" s="23">
-        <f ca="1">IFERROR(R$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="S4" s="23">
-        <f ca="1">IFERROR(S$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="T4" s="24">
-        <f ca="1">IFERROR(T$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AA4" s="6">
@@ -6455,18 +5948,18 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="A30:A32">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:I32">
-    <cfRule type="expression" dxfId="40" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="2" stopIfTrue="1">
       <formula>$A2=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="3" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6502,7 +5995,7 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>March 
@@ -6643,7 +6136,7 @@
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
-        <v>https://d.docs.live.net/76781d05666600c8/Documents/[Modry_Zivot.xlsx]3</v>
+        <v>C:\Users\david.benedeki\Programming\Shared\ModryZivot\[Modry_Zivot.xlsx]3</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -6718,35 +6211,35 @@
         <v>Total %</v>
       </c>
       <c r="M4" s="23">
-        <f ca="1">IFERROR(M$2/$AA4*100, "")</f>
+        <f t="shared" ref="M4:T4" ca="1" si="2">IFERROR(M$2/$AA4*100, "")</f>
         <v>0</v>
       </c>
       <c r="N4" s="23">
-        <f ca="1">IFERROR(N$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="O4" s="23">
-        <f ca="1">IFERROR(O$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="23">
-        <f ca="1">IFERROR(P$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="Q4" s="23">
-        <f ca="1">IFERROR(Q$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="R4" s="23">
-        <f ca="1">IFERROR(R$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="S4" s="23">
-        <f ca="1">IFERROR(S$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="T4" s="24">
-        <f ca="1">IFERROR(T$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AA4" s="6">
@@ -7153,18 +6646,18 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="A30:A32">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:I32">
-    <cfRule type="expression" dxfId="36" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="2" stopIfTrue="1">
       <formula>$A2=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="3" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7200,7 +6693,7 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>April 
@@ -7341,7 +6834,7 @@
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
-        <v>https://d.docs.live.net/76781d05666600c8/Documents/[Modry_Zivot.xlsx]4</v>
+        <v>C:\Users\david.benedeki\Programming\Shared\ModryZivot\[Modry_Zivot.xlsx]4</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -7416,35 +6909,35 @@
         <v>Total %</v>
       </c>
       <c r="M4" s="23">
-        <f ca="1">IFERROR(M$2/$AA4*100, "")</f>
+        <f t="shared" ref="M4:T4" ca="1" si="2">IFERROR(M$2/$AA4*100, "")</f>
         <v>0</v>
       </c>
       <c r="N4" s="23">
-        <f ca="1">IFERROR(N$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="O4" s="23">
-        <f ca="1">IFERROR(O$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="23">
-        <f ca="1">IFERROR(P$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="Q4" s="23">
-        <f ca="1">IFERROR(Q$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="R4" s="23">
-        <f ca="1">IFERROR(R$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="S4" s="23">
-        <f ca="1">IFERROR(S$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="T4" s="24">
-        <f ca="1">IFERROR(T$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AA4" s="6">
@@ -7851,18 +7344,18 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="A30:A32">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:I32">
-    <cfRule type="expression" dxfId="32" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="2" stopIfTrue="1">
       <formula>$A2=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7898,7 +7391,7 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>May 
@@ -8039,7 +7532,7 @@
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
-        <v>https://d.docs.live.net/76781d05666600c8/Documents/[Modry_Zivot.xlsx]5</v>
+        <v>C:\Users\david.benedeki\Programming\Shared\ModryZivot\[Modry_Zivot.xlsx]5</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -8114,35 +7607,35 @@
         <v>Total %</v>
       </c>
       <c r="M4" s="23">
-        <f ca="1">IFERROR(M$2/$AA4*100, "")</f>
+        <f t="shared" ref="M4:T4" ca="1" si="2">IFERROR(M$2/$AA4*100, "")</f>
         <v>0</v>
       </c>
       <c r="N4" s="23">
-        <f ca="1">IFERROR(N$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="O4" s="23">
-        <f ca="1">IFERROR(O$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="23">
-        <f ca="1">IFERROR(P$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="Q4" s="23">
-        <f ca="1">IFERROR(Q$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="R4" s="23">
-        <f ca="1">IFERROR(R$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="S4" s="23">
-        <f ca="1">IFERROR(S$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="T4" s="24">
-        <f ca="1">IFERROR(T$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AA4" s="6">
@@ -8549,18 +8042,18 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="A30:A32">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:I32">
-    <cfRule type="expression" dxfId="28" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="2" stopIfTrue="1">
       <formula>$A2=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8596,7 +8089,7 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>June 
@@ -8737,7 +8230,7 @@
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
-        <v>https://d.docs.live.net/76781d05666600c8/Documents/[Modry_Zivot.xlsx]6</v>
+        <v>C:\Users\david.benedeki\Programming\Shared\ModryZivot\[Modry_Zivot.xlsx]6</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -8812,35 +8305,35 @@
         <v>Total %</v>
       </c>
       <c r="M4" s="23">
-        <f ca="1">IFERROR(M$2/$AA4*100, "")</f>
+        <f t="shared" ref="M4:T4" ca="1" si="2">IFERROR(M$2/$AA4*100, "")</f>
         <v>0</v>
       </c>
       <c r="N4" s="23">
-        <f ca="1">IFERROR(N$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="O4" s="23">
-        <f ca="1">IFERROR(O$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="23">
-        <f ca="1">IFERROR(P$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="Q4" s="23">
-        <f ca="1">IFERROR(Q$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="R4" s="23">
-        <f ca="1">IFERROR(R$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="S4" s="23">
-        <f ca="1">IFERROR(S$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="T4" s="24">
-        <f ca="1">IFERROR(T$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AA4" s="6">
@@ -9247,18 +8740,18 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="A30:A32">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:I32">
-    <cfRule type="expression" dxfId="24" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="2" stopIfTrue="1">
       <formula>$A2=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="3" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9294,7 +8787,7 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>July 
@@ -9435,7 +8928,7 @@
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
-        <v>https://d.docs.live.net/76781d05666600c8/Documents/[Modry_Zivot.xlsx]7</v>
+        <v>C:\Users\david.benedeki\Programming\Shared\ModryZivot\[Modry_Zivot.xlsx]7</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -9510,35 +9003,35 @@
         <v>Total %</v>
       </c>
       <c r="M4" s="23">
-        <f ca="1">IFERROR(M$2/$AA4*100, "")</f>
+        <f t="shared" ref="M4:T4" ca="1" si="2">IFERROR(M$2/$AA4*100, "")</f>
         <v>0</v>
       </c>
       <c r="N4" s="23">
-        <f ca="1">IFERROR(N$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="O4" s="23">
-        <f ca="1">IFERROR(O$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="23">
-        <f ca="1">IFERROR(P$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="Q4" s="23">
-        <f ca="1">IFERROR(Q$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="R4" s="23">
-        <f ca="1">IFERROR(R$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="S4" s="23">
-        <f ca="1">IFERROR(S$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="T4" s="24">
-        <f ca="1">IFERROR(T$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AA4" s="6">
@@ -9945,18 +9438,18 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="A30:A32">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:I32">
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="2" stopIfTrue="1">
       <formula>$A2=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9992,7 +9485,7 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>August 
@@ -10133,7 +9626,7 @@
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
-        <v>https://d.docs.live.net/76781d05666600c8/Documents/[Modry_Zivot.xlsx]8</v>
+        <v>C:\Users\david.benedeki\Programming\Shared\ModryZivot\[Modry_Zivot.xlsx]8</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -10208,35 +9701,35 @@
         <v>Total %</v>
       </c>
       <c r="M4" s="23">
-        <f ca="1">IFERROR(M$2/$AA4*100, "")</f>
+        <f t="shared" ref="M4:T4" ca="1" si="2">IFERROR(M$2/$AA4*100, "")</f>
         <v>0</v>
       </c>
       <c r="N4" s="23">
-        <f ca="1">IFERROR(N$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="O4" s="23">
-        <f ca="1">IFERROR(O$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="23">
-        <f ca="1">IFERROR(P$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="Q4" s="23">
-        <f ca="1">IFERROR(Q$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="R4" s="23">
-        <f ca="1">IFERROR(R$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="S4" s="23">
-        <f ca="1">IFERROR(S$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="T4" s="24">
-        <f ca="1">IFERROR(T$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AA4" s="6">
@@ -10639,15 +10132,15 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="B2:I32">
-    <cfRule type="cellIs" dxfId="68" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="4" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:A32">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10683,7 +10176,7 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>September 
@@ -10820,11 +10313,11 @@
       </c>
       <c r="X2" s="29">
         <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),NOW()&lt;DATE(YEAR,$W$2,1)),0,MIN(NOW(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
-        <v>6.6968726851846441</v>
+        <v>17.724486574072216</v>
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
-        <v>https://d.docs.live.net/76781d05666600c8/Documents/[Modry_Zivot.xlsx]9</v>
+        <v>C:\Users\david.benedeki\Programming\Shared\ModryZivot\[Modry_Zivot.xlsx]9</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -10899,35 +10392,35 @@
         <v>Total %</v>
       </c>
       <c r="M4" s="23">
-        <f ca="1">IFERROR(M$2/$AA4*100, "")</f>
+        <f t="shared" ref="M4:T4" ca="1" si="2">IFERROR(M$2/$AA4*100, "")</f>
         <v>0</v>
       </c>
       <c r="N4" s="23">
-        <f ca="1">IFERROR(N$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="O4" s="23">
-        <f ca="1">IFERROR(O$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="23">
-        <f ca="1">IFERROR(P$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="Q4" s="23">
-        <f ca="1">IFERROR(Q$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="R4" s="23">
-        <f ca="1">IFERROR(R$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="S4" s="23">
-        <f ca="1">IFERROR(S$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="T4" s="24">
-        <f ca="1">IFERROR(T$2/$AA4*100, "")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="AA4" s="6">
@@ -11330,18 +10823,18 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="B2:I32">
-    <cfRule type="expression" dxfId="65" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
       <formula>$A2=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:A32">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Version 1.2 * Fixed a bug, where the current number of days in a month was fractional number, instead of a whole one by using function `TODAY()` instead of `NOW()`
</commit_message>
<xml_diff>
--- a/Modry_Zivot.xlsx
+++ b/Modry_Zivot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.benedeki\Programming\Shared\ModryZivot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80369E4A-BE45-4273-BDFE-3CD653723FE0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8DA3A6-EECB-403E-8F75-BBE1A7BDF32A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23325" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="6" r:id="rId1"/>
@@ -1768,11 +1768,11 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="88.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>January 
- 2019</v>
+ 2020</v>
       </c>
       <c r="B1" s="14" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
@@ -1853,7 +1853,7 @@
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f t="shared" ref="A2:A29" ca="1" si="0">ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")"</f>
-        <v>1. (Tue)</v>
+        <v>1. (Wed)</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1904,8 +1904,8 @@
         <v>1</v>
       </c>
       <c r="X2" s="29">
-        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),NOW()&lt;DATE(YEAR,$W$2,1)),0,MIN(NOW(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
-        <v>31</v>
+        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),TODAY()&lt;DATE(YEAR,$W$2,1)),0,MIN(TODAY(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
+        <v>4</v>
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
@@ -1915,7 +1915,7 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2. (Wed)</v>
+        <v>2. (Thu)</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1963,13 +1963,13 @@
       </c>
       <c r="AA3" s="3">
         <f ca="1">DATE(YEAR,$W$2,1)</f>
-        <v>43466</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3. (Thu)</v>
+        <v>3. (Fri)</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2023,7 +2023,7 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>4. (Fri)</v>
+        <v>4. (Sat)</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2037,7 +2037,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5. (Sat)</v>
+        <v>5. (Sun)</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2051,7 +2051,7 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6. (Sun)</v>
+        <v>6. (Mon)</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -2065,7 +2065,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7. (Mon)</v>
+        <v>7. (Tue)</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2079,7 +2079,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>8. (Tue)</v>
+        <v>8. (Wed)</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2093,7 +2093,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>9. (Wed)</v>
+        <v>9. (Thu)</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2107,7 +2107,7 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10. (Thu)</v>
+        <v>10. (Fri)</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2121,7 +2121,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>11. (Fri)</v>
+        <v>11. (Sat)</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2135,7 +2135,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12. (Sat)</v>
+        <v>12. (Sun)</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2149,7 +2149,7 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13. (Sun)</v>
+        <v>13. (Mon)</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2163,7 +2163,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>14. (Mon)</v>
+        <v>14. (Tue)</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2177,7 +2177,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15. (Tue)</v>
+        <v>15. (Wed)</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2191,7 +2191,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16. (Wed)</v>
+        <v>16. (Thu)</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2205,7 +2205,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17. (Thu)</v>
+        <v>17. (Fri)</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2219,7 +2219,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18. (Fri)</v>
+        <v>18. (Sat)</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -2233,7 +2233,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19. (Sat)</v>
+        <v>19. (Sun)</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -2247,7 +2247,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20. (Sun)</v>
+        <v>20. (Mon)</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -2261,7 +2261,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>21. (Mon)</v>
+        <v>21. (Tue)</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2275,7 +2275,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>22. (Tue)</v>
+        <v>22. (Wed)</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2289,7 +2289,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>23. (Wed)</v>
+        <v>23. (Thu)</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2303,7 +2303,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24. (Thu)</v>
+        <v>24. (Fri)</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2317,7 +2317,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>25. (Fri)</v>
+        <v>25. (Sat)</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2331,7 +2331,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26. (Sat)</v>
+        <v>26. (Sun)</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2345,7 +2345,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>27. (Sun)</v>
+        <v>27. (Mon)</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2359,7 +2359,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>28. (Mon)</v>
+        <v>28. (Tue)</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2373,7 +2373,7 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>29. (Tue)</v>
+        <v>29. (Wed)</v>
       </c>
       <c r="B30" s="4">
         <v>0</v>
@@ -2391,7 +2391,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>30. (Wed)</v>
+        <v>30. (Thu)</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2405,7 +2405,7 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>31. (Thu)</v>
+        <v>31. (Fri)</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2466,11 +2466,11 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="88.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>October 
- 2019</v>
+ 2020</v>
       </c>
       <c r="B1" s="14" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
@@ -2551,7 +2551,7 @@
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f t="shared" ref="A2:A29" ca="1" si="0">ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")"</f>
-        <v>1. (Tue)</v>
+        <v>1. (Thu)</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2602,7 +2602,7 @@
         <v>10</v>
       </c>
       <c r="X2" s="29">
-        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),NOW()&lt;DATE(YEAR,$W$2,1)),0,MIN(NOW(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
+        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),TODAY()&lt;DATE(YEAR,$W$2,1)),0,MIN(TODAY(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
         <v>0</v>
       </c>
       <c r="AA2" s="2" t="str">
@@ -2613,7 +2613,7 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2. (Wed)</v>
+        <v>2. (Fri)</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -2661,13 +2661,13 @@
       </c>
       <c r="AA3" s="3">
         <f ca="1">DATE(YEAR,$W$2,1)</f>
-        <v>43739</v>
+        <v>44105</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3. (Thu)</v>
+        <v>3. (Sat)</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2721,7 +2721,7 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>4. (Fri)</v>
+        <v>4. (Sun)</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2735,7 +2735,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5. (Sat)</v>
+        <v>5. (Mon)</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2749,7 +2749,7 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6. (Sun)</v>
+        <v>6. (Tue)</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -2763,7 +2763,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7. (Mon)</v>
+        <v>7. (Wed)</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2777,7 +2777,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>8. (Tue)</v>
+        <v>8. (Thu)</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2791,7 +2791,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>9. (Wed)</v>
+        <v>9. (Fri)</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2805,7 +2805,7 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10. (Thu)</v>
+        <v>10. (Sat)</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2819,7 +2819,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>11. (Fri)</v>
+        <v>11. (Sun)</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2833,7 +2833,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12. (Sat)</v>
+        <v>12. (Mon)</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2847,7 +2847,7 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13. (Sun)</v>
+        <v>13. (Tue)</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2861,7 +2861,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>14. (Mon)</v>
+        <v>14. (Wed)</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2875,7 +2875,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15. (Tue)</v>
+        <v>15. (Thu)</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2889,7 +2889,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16. (Wed)</v>
+        <v>16. (Fri)</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2903,7 +2903,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17. (Thu)</v>
+        <v>17. (Sat)</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2917,7 +2917,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18. (Fri)</v>
+        <v>18. (Sun)</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -2931,7 +2931,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19. (Sat)</v>
+        <v>19. (Mon)</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -2945,7 +2945,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20. (Sun)</v>
+        <v>20. (Tue)</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -2959,7 +2959,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>21. (Mon)</v>
+        <v>21. (Wed)</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2973,7 +2973,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>22. (Tue)</v>
+        <v>22. (Thu)</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2987,7 +2987,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>23. (Wed)</v>
+        <v>23. (Fri)</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -3001,7 +3001,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24. (Thu)</v>
+        <v>24. (Sat)</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3015,7 +3015,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>25. (Fri)</v>
+        <v>25. (Sun)</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3029,7 +3029,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26. (Sat)</v>
+        <v>26. (Mon)</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -3043,7 +3043,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>27. (Sun)</v>
+        <v>27. (Tue)</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -3057,7 +3057,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>28. (Mon)</v>
+        <v>28. (Wed)</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -3071,7 +3071,7 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>29. (Tue)</v>
+        <v>29. (Thu)</v>
       </c>
       <c r="B30" s="4">
         <v>0</v>
@@ -3089,7 +3089,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>30. (Wed)</v>
+        <v>30. (Fri)</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -3103,7 +3103,7 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>31. (Thu)</v>
+        <v>31. (Sat)</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -3164,11 +3164,11 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="88.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>November 
- 2019</v>
+ 2020</v>
       </c>
       <c r="B1" s="14" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
@@ -3249,7 +3249,7 @@
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f t="shared" ref="A2:A29" ca="1" si="0">ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")"</f>
-        <v>1. (Fri)</v>
+        <v>1. (Sun)</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3300,7 +3300,7 @@
         <v>11</v>
       </c>
       <c r="X2" s="29">
-        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),NOW()&lt;DATE(YEAR,$W$2,1)),0,MIN(NOW(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
+        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),TODAY()&lt;DATE(YEAR,$W$2,1)),0,MIN(TODAY(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
         <v>0</v>
       </c>
       <c r="AA2" s="2" t="str">
@@ -3311,7 +3311,7 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2. (Sat)</v>
+        <v>2. (Mon)</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3359,13 +3359,13 @@
       </c>
       <c r="AA3" s="3">
         <f ca="1">DATE(YEAR,$W$2,1)</f>
-        <v>43770</v>
+        <v>44136</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3. (Sun)</v>
+        <v>3. (Tue)</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3419,7 +3419,7 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>4. (Mon)</v>
+        <v>4. (Wed)</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -3433,7 +3433,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5. (Tue)</v>
+        <v>5. (Thu)</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -3447,7 +3447,7 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6. (Wed)</v>
+        <v>6. (Fri)</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3461,7 +3461,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7. (Thu)</v>
+        <v>7. (Sat)</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -3475,7 +3475,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>8. (Fri)</v>
+        <v>8. (Sun)</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -3489,7 +3489,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>9. (Sat)</v>
+        <v>9. (Mon)</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -3503,7 +3503,7 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10. (Sun)</v>
+        <v>10. (Tue)</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -3517,7 +3517,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>11. (Mon)</v>
+        <v>11. (Wed)</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -3531,7 +3531,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12. (Tue)</v>
+        <v>12. (Thu)</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -3545,7 +3545,7 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13. (Wed)</v>
+        <v>13. (Fri)</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -3559,7 +3559,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>14. (Thu)</v>
+        <v>14. (Sat)</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -3573,7 +3573,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15. (Fri)</v>
+        <v>15. (Sun)</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -3587,7 +3587,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16. (Sat)</v>
+        <v>16. (Mon)</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -3601,7 +3601,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17. (Sun)</v>
+        <v>17. (Tue)</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -3615,7 +3615,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18. (Mon)</v>
+        <v>18. (Wed)</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -3629,7 +3629,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19. (Tue)</v>
+        <v>19. (Thu)</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -3643,7 +3643,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20. (Wed)</v>
+        <v>20. (Fri)</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -3657,7 +3657,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>21. (Thu)</v>
+        <v>21. (Sat)</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -3671,7 +3671,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>22. (Fri)</v>
+        <v>22. (Sun)</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3685,7 +3685,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>23. (Sat)</v>
+        <v>23. (Mon)</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -3699,7 +3699,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24. (Sun)</v>
+        <v>24. (Tue)</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3713,7 +3713,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>25. (Mon)</v>
+        <v>25. (Wed)</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3727,7 +3727,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26. (Tue)</v>
+        <v>26. (Thu)</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -3741,7 +3741,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>27. (Wed)</v>
+        <v>27. (Fri)</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -3755,7 +3755,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>28. (Thu)</v>
+        <v>28. (Sat)</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -3769,7 +3769,7 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>29. (Fri)</v>
+        <v>29. (Sun)</v>
       </c>
       <c r="B30" s="4">
         <v>0</v>
@@ -3787,7 +3787,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>30. (Sat)</v>
+        <v>30. (Mon)</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -3862,11 +3862,11 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="88.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>December 
- 2019</v>
+ 2020</v>
       </c>
       <c r="B1" s="14" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
@@ -3947,7 +3947,7 @@
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f t="shared" ref="A2:A29" ca="1" si="0">ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")"</f>
-        <v>1. (Sun)</v>
+        <v>1. (Tue)</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3998,7 +3998,7 @@
         <v>12</v>
       </c>
       <c r="X2" s="29">
-        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),NOW()&lt;DATE(YEAR,$W$2,1)),0,MIN(NOW(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
+        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),TODAY()&lt;DATE(YEAR,$W$2,1)),0,MIN(TODAY(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
         <v>0</v>
       </c>
       <c r="AA2" s="2" t="str">
@@ -4009,7 +4009,7 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2. (Mon)</v>
+        <v>2. (Wed)</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -4057,13 +4057,13 @@
       </c>
       <c r="AA3" s="3">
         <f ca="1">DATE(YEAR,$W$2,1)</f>
-        <v>43800</v>
+        <v>44166</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3. (Tue)</v>
+        <v>3. (Thu)</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -4117,7 +4117,7 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>4. (Wed)</v>
+        <v>4. (Fri)</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -4131,7 +4131,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5. (Thu)</v>
+        <v>5. (Sat)</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -4145,7 +4145,7 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6. (Fri)</v>
+        <v>6. (Sun)</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -4159,7 +4159,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7. (Sat)</v>
+        <v>7. (Mon)</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -4173,7 +4173,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>8. (Sun)</v>
+        <v>8. (Tue)</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -4187,7 +4187,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>9. (Mon)</v>
+        <v>9. (Wed)</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -4201,7 +4201,7 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10. (Tue)</v>
+        <v>10. (Thu)</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -4215,7 +4215,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>11. (Wed)</v>
+        <v>11. (Fri)</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -4229,7 +4229,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12. (Thu)</v>
+        <v>12. (Sat)</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -4243,7 +4243,7 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13. (Fri)</v>
+        <v>13. (Sun)</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -4257,7 +4257,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>14. (Sat)</v>
+        <v>14. (Mon)</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -4271,7 +4271,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15. (Sun)</v>
+        <v>15. (Tue)</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -4285,7 +4285,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16. (Mon)</v>
+        <v>16. (Wed)</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -4299,7 +4299,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17. (Tue)</v>
+        <v>17. (Thu)</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -4313,7 +4313,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18. (Wed)</v>
+        <v>18. (Fri)</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -4327,7 +4327,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19. (Thu)</v>
+        <v>19. (Sat)</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -4341,7 +4341,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20. (Fri)</v>
+        <v>20. (Sun)</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -4355,7 +4355,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>21. (Sat)</v>
+        <v>21. (Mon)</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -4369,7 +4369,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>22. (Sun)</v>
+        <v>22. (Tue)</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -4383,7 +4383,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>23. (Mon)</v>
+        <v>23. (Wed)</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -4397,7 +4397,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24. (Tue)</v>
+        <v>24. (Thu)</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -4411,7 +4411,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>25. (Wed)</v>
+        <v>25. (Fri)</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -4425,7 +4425,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26. (Thu)</v>
+        <v>26. (Sat)</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -4439,7 +4439,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>27. (Fri)</v>
+        <v>27. (Sun)</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -4453,7 +4453,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>28. (Sat)</v>
+        <v>28. (Mon)</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -4467,7 +4467,7 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>29. (Sun)</v>
+        <v>29. (Tue)</v>
       </c>
       <c r="B30" s="4">
         <v>0</v>
@@ -4485,7 +4485,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>30. (Mon)</v>
+        <v>30. (Wed)</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -4499,7 +4499,7 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>31. (Tue)</v>
+        <v>31. (Thu)</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -4543,7 +4543,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4560,7 +4560,7 @@
     <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="87.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="88.5" x14ac:dyDescent="0.25">
       <c r="F1" s="25" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
         <v>Teeth brushing</v>
@@ -4656,11 +4656,11 @@
       </c>
       <c r="P2" s="48">
         <f ca="1">'1'!X2+'2'!X2+'3'!X2+'4'!X2+'5'!X2+'6'!X2+'7'!X2+'8'!X2+'9'!X2+'10'!X2+'11'!X2+'12'!X2</f>
-        <v>260.72448657407222</v>
+        <v>4</v>
       </c>
       <c r="Q2" s="49">
         <f ca="1">'1'!AA4+'2'!AA4+'3'!AA4+'4'!AA4+'5'!AA4+'6'!AA4+'7'!AA4+'8'!AA4+'9'!AA4+'10'!AA4+'11'!AA4+'12'!AA4</f>
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -4669,7 +4669,7 @@
         <v>Year</v>
       </c>
       <c r="B3" s="31">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="E3" s="34" t="str">
         <f ca="1">E2&amp;" %"</f>
@@ -4719,7 +4719,7 @@
       </c>
       <c r="B4" s="32">
         <f>DATE(YEAR,1,1)</f>
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="E4" s="35" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,26,4,1,TRANS_SH))&amp;" %"</f>
@@ -4730,7 +4730,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="46">
-        <f t="shared" ref="G4:N4" ca="1" si="1">100*G$2/$Q2</f>
+        <f t="shared" ref="G4:M4" ca="1" si="1">100*G$2/$Q2</f>
         <v>0</v>
       </c>
       <c r="H4" s="46">
@@ -4768,7 +4768,7 @@
         <v>Version</v>
       </c>
       <c r="B5" s="36">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -4794,6 +4794,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{C44B8540-8AD2-4EFD-919F-C5EAD4CE8BDB}">
       <formula1>LANGUAGES</formula1>
@@ -5297,11 +5298,11 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="88.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>Ferbuary 
- 2019</v>
+ 2020</v>
       </c>
       <c r="B1" s="14" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
@@ -5382,7 +5383,7 @@
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f t="shared" ref="A2:A29" ca="1" si="0">ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")"</f>
-        <v>1. (Fri)</v>
+        <v>1. (Sat)</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -5433,8 +5434,8 @@
         <v>2</v>
       </c>
       <c r="X2" s="29">
-        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),NOW()&lt;DATE(YEAR,$W$2,1)),0,MIN(NOW(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
-        <v>28</v>
+        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),TODAY()&lt;DATE(YEAR,$W$2,1)),0,MIN(TODAY(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
+        <v>0</v>
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
@@ -5444,7 +5445,7 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2. (Sat)</v>
+        <v>2. (Sun)</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -5458,47 +5459,47 @@
         <f ca="1">L2&amp;" %"</f>
         <v>Current %</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="20" t="str">
         <f ca="1">IFERROR(M$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="20">
+        <v/>
+      </c>
+      <c r="N3" s="20" t="str">
         <f t="shared" ref="N3:T3" ca="1" si="1">IFERROR(N$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="20">
+        <v/>
+      </c>
+      <c r="O3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="20">
+        <v/>
+      </c>
+      <c r="P3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="20">
+        <v/>
+      </c>
+      <c r="Q3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R3" s="20">
+        <v/>
+      </c>
+      <c r="R3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S3" s="20">
+        <v/>
+      </c>
+      <c r="S3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T3" s="21">
+        <v/>
+      </c>
+      <c r="T3" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AA3" s="3">
         <f ca="1">DATE(YEAR,$W$2,1)</f>
-        <v>43497</v>
+        <v>43862</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3. (Sun)</v>
+        <v>3. (Mon)</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -5546,13 +5547,13 @@
       </c>
       <c r="AA4" s="6">
         <f ca="1">_xlfn.DAYS(EOMONTH(AA3,0),AA3)+1</f>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>4. (Mon)</v>
+        <v>4. (Tue)</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -5566,7 +5567,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5. (Tue)</v>
+        <v>5. (Wed)</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -5580,7 +5581,7 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6. (Wed)</v>
+        <v>6. (Thu)</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -5594,7 +5595,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7. (Thu)</v>
+        <v>7. (Fri)</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -5608,7 +5609,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>8. (Fri)</v>
+        <v>8. (Sat)</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -5622,7 +5623,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>9. (Sat)</v>
+        <v>9. (Sun)</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -5636,7 +5637,7 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10. (Sun)</v>
+        <v>10. (Mon)</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -5650,7 +5651,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>11. (Mon)</v>
+        <v>11. (Tue)</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -5664,7 +5665,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12. (Tue)</v>
+        <v>12. (Wed)</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -5678,7 +5679,7 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13. (Wed)</v>
+        <v>13. (Thu)</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -5692,7 +5693,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>14. (Thu)</v>
+        <v>14. (Fri)</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -5706,7 +5707,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15. (Fri)</v>
+        <v>15. (Sat)</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -5720,7 +5721,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16. (Sat)</v>
+        <v>16. (Sun)</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -5734,7 +5735,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17. (Sun)</v>
+        <v>17. (Mon)</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -5748,7 +5749,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18. (Mon)</v>
+        <v>18. (Tue)</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -5762,7 +5763,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19. (Tue)</v>
+        <v>19. (Wed)</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -5776,7 +5777,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20. (Wed)</v>
+        <v>20. (Thu)</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -5790,7 +5791,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>21. (Thu)</v>
+        <v>21. (Fri)</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -5804,7 +5805,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>22. (Fri)</v>
+        <v>22. (Sat)</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -5818,7 +5819,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>23. (Sat)</v>
+        <v>23. (Sun)</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -5832,7 +5833,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24. (Sun)</v>
+        <v>24. (Mon)</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -5846,7 +5847,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>25. (Mon)</v>
+        <v>25. (Tue)</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -5860,7 +5861,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26. (Tue)</v>
+        <v>26. (Wed)</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -5874,7 +5875,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>27. (Wed)</v>
+        <v>27. (Thu)</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -5888,7 +5889,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>28. (Thu)</v>
+        <v>28. (Fri)</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -5902,7 +5903,7 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v/>
+        <v>29. (Sat)</v>
       </c>
       <c r="B30" s="4">
         <v>0</v>
@@ -5995,11 +5996,11 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="88.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>March 
- 2019</v>
+ 2020</v>
       </c>
       <c r="B1" s="14" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
@@ -6080,7 +6081,7 @@
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f t="shared" ref="A2:A29" ca="1" si="0">ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")"</f>
-        <v>1. (Fri)</v>
+        <v>1. (Sun)</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -6131,8 +6132,8 @@
         <v>3</v>
       </c>
       <c r="X2" s="29">
-        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),NOW()&lt;DATE(YEAR,$W$2,1)),0,MIN(NOW(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
-        <v>31</v>
+        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),TODAY()&lt;DATE(YEAR,$W$2,1)),0,MIN(TODAY(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
+        <v>0</v>
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
@@ -6142,7 +6143,7 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2. (Sat)</v>
+        <v>2. (Mon)</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -6156,47 +6157,47 @@
         <f ca="1">L2&amp;" %"</f>
         <v>Current %</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="20" t="str">
         <f ca="1">IFERROR(M$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="20">
+        <v/>
+      </c>
+      <c r="N3" s="20" t="str">
         <f t="shared" ref="N3:T3" ca="1" si="1">IFERROR(N$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="20">
+        <v/>
+      </c>
+      <c r="O3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="20">
+        <v/>
+      </c>
+      <c r="P3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="20">
+        <v/>
+      </c>
+      <c r="Q3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R3" s="20">
+        <v/>
+      </c>
+      <c r="R3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S3" s="20">
+        <v/>
+      </c>
+      <c r="S3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T3" s="21">
+        <v/>
+      </c>
+      <c r="T3" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AA3" s="3">
         <f ca="1">DATE(YEAR,$W$2,1)</f>
-        <v>43525</v>
+        <v>43891</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3. (Sun)</v>
+        <v>3. (Tue)</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -6250,7 +6251,7 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>4. (Mon)</v>
+        <v>4. (Wed)</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -6264,7 +6265,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5. (Tue)</v>
+        <v>5. (Thu)</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -6278,7 +6279,7 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6. (Wed)</v>
+        <v>6. (Fri)</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -6292,7 +6293,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7. (Thu)</v>
+        <v>7. (Sat)</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -6306,7 +6307,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>8. (Fri)</v>
+        <v>8. (Sun)</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -6320,7 +6321,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>9. (Sat)</v>
+        <v>9. (Mon)</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -6334,7 +6335,7 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10. (Sun)</v>
+        <v>10. (Tue)</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -6348,7 +6349,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>11. (Mon)</v>
+        <v>11. (Wed)</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -6362,7 +6363,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12. (Tue)</v>
+        <v>12. (Thu)</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -6376,7 +6377,7 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13. (Wed)</v>
+        <v>13. (Fri)</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -6390,7 +6391,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>14. (Thu)</v>
+        <v>14. (Sat)</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -6404,7 +6405,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15. (Fri)</v>
+        <v>15. (Sun)</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -6418,7 +6419,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16. (Sat)</v>
+        <v>16. (Mon)</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -6432,7 +6433,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17. (Sun)</v>
+        <v>17. (Tue)</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -6446,7 +6447,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18. (Mon)</v>
+        <v>18. (Wed)</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -6460,7 +6461,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19. (Tue)</v>
+        <v>19. (Thu)</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -6474,7 +6475,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20. (Wed)</v>
+        <v>20. (Fri)</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -6488,7 +6489,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>21. (Thu)</v>
+        <v>21. (Sat)</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -6502,7 +6503,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>22. (Fri)</v>
+        <v>22. (Sun)</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -6516,7 +6517,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>23. (Sat)</v>
+        <v>23. (Mon)</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -6530,7 +6531,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24. (Sun)</v>
+        <v>24. (Tue)</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -6544,7 +6545,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>25. (Mon)</v>
+        <v>25. (Wed)</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -6558,7 +6559,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26. (Tue)</v>
+        <v>26. (Thu)</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -6572,7 +6573,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>27. (Wed)</v>
+        <v>27. (Fri)</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -6586,7 +6587,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>28. (Thu)</v>
+        <v>28. (Sat)</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -6600,7 +6601,7 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>29. (Fri)</v>
+        <v>29. (Sun)</v>
       </c>
       <c r="B30" s="4">
         <v>0</v>
@@ -6618,7 +6619,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>30. (Sat)</v>
+        <v>30. (Mon)</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -6632,7 +6633,7 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>31. (Sun)</v>
+        <v>31. (Tue)</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -6693,11 +6694,11 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="88.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>April 
- 2019</v>
+ 2020</v>
       </c>
       <c r="B1" s="14" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
@@ -6778,7 +6779,7 @@
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f t="shared" ref="A2:A29" ca="1" si="0">ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")"</f>
-        <v>1. (Mon)</v>
+        <v>1. (Wed)</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -6829,8 +6830,8 @@
         <v>4</v>
       </c>
       <c r="X2" s="29">
-        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),NOW()&lt;DATE(YEAR,$W$2,1)),0,MIN(NOW(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
-        <v>30</v>
+        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),TODAY()&lt;DATE(YEAR,$W$2,1)),0,MIN(TODAY(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
+        <v>0</v>
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
@@ -6840,7 +6841,7 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2. (Tue)</v>
+        <v>2. (Thu)</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -6854,47 +6855,47 @@
         <f ca="1">L2&amp;" %"</f>
         <v>Current %</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="20" t="str">
         <f ca="1">IFERROR(M$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="20">
+        <v/>
+      </c>
+      <c r="N3" s="20" t="str">
         <f t="shared" ref="N3:T3" ca="1" si="1">IFERROR(N$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="20">
+        <v/>
+      </c>
+      <c r="O3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="20">
+        <v/>
+      </c>
+      <c r="P3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="20">
+        <v/>
+      </c>
+      <c r="Q3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R3" s="20">
+        <v/>
+      </c>
+      <c r="R3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S3" s="20">
+        <v/>
+      </c>
+      <c r="S3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T3" s="21">
+        <v/>
+      </c>
+      <c r="T3" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AA3" s="3">
         <f ca="1">DATE(YEAR,$W$2,1)</f>
-        <v>43556</v>
+        <v>43922</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3. (Wed)</v>
+        <v>3. (Fri)</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -6948,7 +6949,7 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>4. (Thu)</v>
+        <v>4. (Sat)</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -6962,7 +6963,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5. (Fri)</v>
+        <v>5. (Sun)</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -6976,7 +6977,7 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6. (Sat)</v>
+        <v>6. (Mon)</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -6990,7 +6991,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7. (Sun)</v>
+        <v>7. (Tue)</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -7004,7 +7005,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>8. (Mon)</v>
+        <v>8. (Wed)</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -7018,7 +7019,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>9. (Tue)</v>
+        <v>9. (Thu)</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -7032,7 +7033,7 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10. (Wed)</v>
+        <v>10. (Fri)</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -7046,7 +7047,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>11. (Thu)</v>
+        <v>11. (Sat)</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -7060,7 +7061,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12. (Fri)</v>
+        <v>12. (Sun)</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -7074,7 +7075,7 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13. (Sat)</v>
+        <v>13. (Mon)</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -7088,7 +7089,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>14. (Sun)</v>
+        <v>14. (Tue)</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -7102,7 +7103,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15. (Mon)</v>
+        <v>15. (Wed)</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -7116,7 +7117,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16. (Tue)</v>
+        <v>16. (Thu)</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -7130,7 +7131,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17. (Wed)</v>
+        <v>17. (Fri)</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -7144,7 +7145,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18. (Thu)</v>
+        <v>18. (Sat)</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -7158,7 +7159,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19. (Fri)</v>
+        <v>19. (Sun)</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -7172,7 +7173,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20. (Sat)</v>
+        <v>20. (Mon)</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -7186,7 +7187,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>21. (Sun)</v>
+        <v>21. (Tue)</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -7200,7 +7201,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>22. (Mon)</v>
+        <v>22. (Wed)</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -7214,7 +7215,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>23. (Tue)</v>
+        <v>23. (Thu)</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -7228,7 +7229,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24. (Wed)</v>
+        <v>24. (Fri)</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -7242,7 +7243,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>25. (Thu)</v>
+        <v>25. (Sat)</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -7256,7 +7257,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26. (Fri)</v>
+        <v>26. (Sun)</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -7270,7 +7271,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>27. (Sat)</v>
+        <v>27. (Mon)</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -7284,7 +7285,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>28. (Sun)</v>
+        <v>28. (Tue)</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -7298,7 +7299,7 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>29. (Mon)</v>
+        <v>29. (Wed)</v>
       </c>
       <c r="B30" s="4">
         <v>0</v>
@@ -7316,7 +7317,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>30. (Tue)</v>
+        <v>30. (Thu)</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -7391,11 +7392,11 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="88.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>May 
- 2019</v>
+ 2020</v>
       </c>
       <c r="B1" s="14" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
@@ -7476,7 +7477,7 @@
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f t="shared" ref="A2:A29" ca="1" si="0">ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")"</f>
-        <v>1. (Wed)</v>
+        <v>1. (Fri)</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -7527,8 +7528,8 @@
         <v>5</v>
       </c>
       <c r="X2" s="29">
-        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),NOW()&lt;DATE(YEAR,$W$2,1)),0,MIN(NOW(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
-        <v>31</v>
+        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),TODAY()&lt;DATE(YEAR,$W$2,1)),0,MIN(TODAY(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
+        <v>0</v>
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
@@ -7538,7 +7539,7 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2. (Thu)</v>
+        <v>2. (Sat)</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -7552,47 +7553,47 @@
         <f ca="1">L2&amp;" %"</f>
         <v>Current %</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="20" t="str">
         <f ca="1">IFERROR(M$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="20">
+        <v/>
+      </c>
+      <c r="N3" s="20" t="str">
         <f t="shared" ref="N3:T3" ca="1" si="1">IFERROR(N$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="20">
+        <v/>
+      </c>
+      <c r="O3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="20">
+        <v/>
+      </c>
+      <c r="P3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="20">
+        <v/>
+      </c>
+      <c r="Q3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R3" s="20">
+        <v/>
+      </c>
+      <c r="R3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S3" s="20">
+        <v/>
+      </c>
+      <c r="S3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T3" s="21">
+        <v/>
+      </c>
+      <c r="T3" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AA3" s="3">
         <f ca="1">DATE(YEAR,$W$2,1)</f>
-        <v>43586</v>
+        <v>43952</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3. (Fri)</v>
+        <v>3. (Sun)</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -7646,7 +7647,7 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>4. (Sat)</v>
+        <v>4. (Mon)</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -7660,7 +7661,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5. (Sun)</v>
+        <v>5. (Tue)</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -7674,7 +7675,7 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6. (Mon)</v>
+        <v>6. (Wed)</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -7688,7 +7689,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7. (Tue)</v>
+        <v>7. (Thu)</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -7702,7 +7703,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>8. (Wed)</v>
+        <v>8. (Fri)</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -7716,7 +7717,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>9. (Thu)</v>
+        <v>9. (Sat)</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -7730,7 +7731,7 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10. (Fri)</v>
+        <v>10. (Sun)</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -7744,7 +7745,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>11. (Sat)</v>
+        <v>11. (Mon)</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -7758,7 +7759,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12. (Sun)</v>
+        <v>12. (Tue)</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -7772,7 +7773,7 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13. (Mon)</v>
+        <v>13. (Wed)</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -7786,7 +7787,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>14. (Tue)</v>
+        <v>14. (Thu)</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -7800,7 +7801,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15. (Wed)</v>
+        <v>15. (Fri)</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -7814,7 +7815,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16. (Thu)</v>
+        <v>16. (Sat)</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -7828,7 +7829,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17. (Fri)</v>
+        <v>17. (Sun)</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -7842,7 +7843,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18. (Sat)</v>
+        <v>18. (Mon)</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -7856,7 +7857,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19. (Sun)</v>
+        <v>19. (Tue)</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -7870,7 +7871,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20. (Mon)</v>
+        <v>20. (Wed)</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -7884,7 +7885,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>21. (Tue)</v>
+        <v>21. (Thu)</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -7898,7 +7899,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>22. (Wed)</v>
+        <v>22. (Fri)</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -7912,7 +7913,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>23. (Thu)</v>
+        <v>23. (Sat)</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -7926,7 +7927,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24. (Fri)</v>
+        <v>24. (Sun)</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -7940,7 +7941,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>25. (Sat)</v>
+        <v>25. (Mon)</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -7954,7 +7955,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26. (Sun)</v>
+        <v>26. (Tue)</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -7968,7 +7969,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>27. (Mon)</v>
+        <v>27. (Wed)</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -7982,7 +7983,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>28. (Tue)</v>
+        <v>28. (Thu)</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -7996,7 +7997,7 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>29. (Wed)</v>
+        <v>29. (Fri)</v>
       </c>
       <c r="B30" s="4">
         <v>0</v>
@@ -8014,7 +8015,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>30. (Thu)</v>
+        <v>30. (Sat)</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -8028,7 +8029,7 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>31. (Fri)</v>
+        <v>31. (Sun)</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -8089,11 +8090,11 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="88.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>June 
- 2019</v>
+ 2020</v>
       </c>
       <c r="B1" s="14" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
@@ -8174,7 +8175,7 @@
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f t="shared" ref="A2:A29" ca="1" si="0">ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")"</f>
-        <v>1. (Sat)</v>
+        <v>1. (Mon)</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -8225,8 +8226,8 @@
         <v>6</v>
       </c>
       <c r="X2" s="29">
-        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),NOW()&lt;DATE(YEAR,$W$2,1)),0,MIN(NOW(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
-        <v>30</v>
+        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),TODAY()&lt;DATE(YEAR,$W$2,1)),0,MIN(TODAY(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
+        <v>0</v>
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
@@ -8236,7 +8237,7 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2. (Sun)</v>
+        <v>2. (Tue)</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -8250,47 +8251,47 @@
         <f ca="1">L2&amp;" %"</f>
         <v>Current %</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="20" t="str">
         <f ca="1">IFERROR(M$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="20">
+        <v/>
+      </c>
+      <c r="N3" s="20" t="str">
         <f t="shared" ref="N3:T3" ca="1" si="1">IFERROR(N$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="20">
+        <v/>
+      </c>
+      <c r="O3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="20">
+        <v/>
+      </c>
+      <c r="P3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="20">
+        <v/>
+      </c>
+      <c r="Q3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R3" s="20">
+        <v/>
+      </c>
+      <c r="R3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S3" s="20">
+        <v/>
+      </c>
+      <c r="S3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T3" s="21">
+        <v/>
+      </c>
+      <c r="T3" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AA3" s="3">
         <f ca="1">DATE(YEAR,$W$2,1)</f>
-        <v>43617</v>
+        <v>43983</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3. (Mon)</v>
+        <v>3. (Wed)</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -8344,7 +8345,7 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>4. (Tue)</v>
+        <v>4. (Thu)</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -8358,7 +8359,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5. (Wed)</v>
+        <v>5. (Fri)</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -8372,7 +8373,7 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6. (Thu)</v>
+        <v>6. (Sat)</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -8386,7 +8387,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7. (Fri)</v>
+        <v>7. (Sun)</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -8400,7 +8401,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>8. (Sat)</v>
+        <v>8. (Mon)</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -8414,7 +8415,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>9. (Sun)</v>
+        <v>9. (Tue)</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -8428,7 +8429,7 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10. (Mon)</v>
+        <v>10. (Wed)</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -8442,7 +8443,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>11. (Tue)</v>
+        <v>11. (Thu)</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -8456,7 +8457,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12. (Wed)</v>
+        <v>12. (Fri)</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -8470,7 +8471,7 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13. (Thu)</v>
+        <v>13. (Sat)</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -8484,7 +8485,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>14. (Fri)</v>
+        <v>14. (Sun)</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -8498,7 +8499,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15. (Sat)</v>
+        <v>15. (Mon)</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -8512,7 +8513,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16. (Sun)</v>
+        <v>16. (Tue)</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -8526,7 +8527,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17. (Mon)</v>
+        <v>17. (Wed)</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -8540,7 +8541,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18. (Tue)</v>
+        <v>18. (Thu)</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -8554,7 +8555,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19. (Wed)</v>
+        <v>19. (Fri)</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -8568,7 +8569,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20. (Thu)</v>
+        <v>20. (Sat)</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -8582,7 +8583,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>21. (Fri)</v>
+        <v>21. (Sun)</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -8596,7 +8597,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>22. (Sat)</v>
+        <v>22. (Mon)</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -8610,7 +8611,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>23. (Sun)</v>
+        <v>23. (Tue)</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -8624,7 +8625,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24. (Mon)</v>
+        <v>24. (Wed)</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -8638,7 +8639,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>25. (Tue)</v>
+        <v>25. (Thu)</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -8652,7 +8653,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26. (Wed)</v>
+        <v>26. (Fri)</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -8666,7 +8667,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>27. (Thu)</v>
+        <v>27. (Sat)</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -8680,7 +8681,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>28. (Fri)</v>
+        <v>28. (Sun)</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -8694,7 +8695,7 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>29. (Sat)</v>
+        <v>29. (Mon)</v>
       </c>
       <c r="B30" s="4">
         <v>0</v>
@@ -8712,7 +8713,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>30. (Sun)</v>
+        <v>30. (Tue)</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -8787,11 +8788,11 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="88.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>July 
- 2019</v>
+ 2020</v>
       </c>
       <c r="B1" s="14" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
@@ -8872,7 +8873,7 @@
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f t="shared" ref="A2:A29" ca="1" si="0">ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")"</f>
-        <v>1. (Mon)</v>
+        <v>1. (Wed)</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -8923,8 +8924,8 @@
         <v>7</v>
       </c>
       <c r="X2" s="29">
-        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),NOW()&lt;DATE(YEAR,$W$2,1)),0,MIN(NOW(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
-        <v>31</v>
+        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),TODAY()&lt;DATE(YEAR,$W$2,1)),0,MIN(TODAY(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
+        <v>0</v>
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
@@ -8934,7 +8935,7 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2. (Tue)</v>
+        <v>2. (Thu)</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -8948,47 +8949,47 @@
         <f ca="1">L2&amp;" %"</f>
         <v>Current %</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="20" t="str">
         <f ca="1">IFERROR(M$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="20">
+        <v/>
+      </c>
+      <c r="N3" s="20" t="str">
         <f t="shared" ref="N3:T3" ca="1" si="1">IFERROR(N$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="20">
+        <v/>
+      </c>
+      <c r="O3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="20">
+        <v/>
+      </c>
+      <c r="P3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="20">
+        <v/>
+      </c>
+      <c r="Q3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R3" s="20">
+        <v/>
+      </c>
+      <c r="R3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S3" s="20">
+        <v/>
+      </c>
+      <c r="S3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T3" s="21">
+        <v/>
+      </c>
+      <c r="T3" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AA3" s="3">
         <f ca="1">DATE(YEAR,$W$2,1)</f>
-        <v>43647</v>
+        <v>44013</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3. (Wed)</v>
+        <v>3. (Fri)</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -9042,7 +9043,7 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>4. (Thu)</v>
+        <v>4. (Sat)</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -9056,7 +9057,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5. (Fri)</v>
+        <v>5. (Sun)</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -9070,7 +9071,7 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6. (Sat)</v>
+        <v>6. (Mon)</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -9084,7 +9085,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7. (Sun)</v>
+        <v>7. (Tue)</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -9098,7 +9099,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>8. (Mon)</v>
+        <v>8. (Wed)</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -9112,7 +9113,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>9. (Tue)</v>
+        <v>9. (Thu)</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -9126,7 +9127,7 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10. (Wed)</v>
+        <v>10. (Fri)</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -9140,7 +9141,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>11. (Thu)</v>
+        <v>11. (Sat)</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -9154,7 +9155,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12. (Fri)</v>
+        <v>12. (Sun)</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -9168,7 +9169,7 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13. (Sat)</v>
+        <v>13. (Mon)</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -9182,7 +9183,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>14. (Sun)</v>
+        <v>14. (Tue)</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -9196,7 +9197,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15. (Mon)</v>
+        <v>15. (Wed)</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -9210,7 +9211,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16. (Tue)</v>
+        <v>16. (Thu)</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -9224,7 +9225,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17. (Wed)</v>
+        <v>17. (Fri)</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -9238,7 +9239,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18. (Thu)</v>
+        <v>18. (Sat)</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -9252,7 +9253,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19. (Fri)</v>
+        <v>19. (Sun)</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -9266,7 +9267,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20. (Sat)</v>
+        <v>20. (Mon)</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -9280,7 +9281,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>21. (Sun)</v>
+        <v>21. (Tue)</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -9294,7 +9295,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>22. (Mon)</v>
+        <v>22. (Wed)</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -9308,7 +9309,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>23. (Tue)</v>
+        <v>23. (Thu)</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -9322,7 +9323,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24. (Wed)</v>
+        <v>24. (Fri)</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -9336,7 +9337,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>25. (Thu)</v>
+        <v>25. (Sat)</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -9350,7 +9351,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26. (Fri)</v>
+        <v>26. (Sun)</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -9364,7 +9365,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>27. (Sat)</v>
+        <v>27. (Mon)</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -9378,7 +9379,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>28. (Sun)</v>
+        <v>28. (Tue)</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -9392,7 +9393,7 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>29. (Mon)</v>
+        <v>29. (Wed)</v>
       </c>
       <c r="B30" s="4">
         <v>0</v>
@@ -9410,7 +9411,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>30. (Tue)</v>
+        <v>30. (Thu)</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -9424,7 +9425,7 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>31. (Wed)</v>
+        <v>31. (Fri)</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -9485,11 +9486,11 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="88.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>August 
- 2019</v>
+ 2020</v>
       </c>
       <c r="B1" s="14" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
@@ -9570,7 +9571,7 @@
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f t="shared" ref="A2:A29" ca="1" si="0">ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")"</f>
-        <v>1. (Thu)</v>
+        <v>1. (Sat)</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -9621,8 +9622,8 @@
         <v>8</v>
       </c>
       <c r="X2" s="29">
-        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),NOW()&lt;DATE(YEAR,$W$2,1)),0,MIN(NOW(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
-        <v>31</v>
+        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),TODAY()&lt;DATE(YEAR,$W$2,1)),0,MIN(TODAY(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
+        <v>0</v>
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
@@ -9632,7 +9633,7 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2. (Fri)</v>
+        <v>2. (Sun)</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -9646,47 +9647,47 @@
         <f ca="1">L2&amp;" %"</f>
         <v>Current %</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="20" t="str">
         <f ca="1">IFERROR(M$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="20">
+        <v/>
+      </c>
+      <c r="N3" s="20" t="str">
         <f t="shared" ref="N3:T3" ca="1" si="1">IFERROR(N$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="20">
+        <v/>
+      </c>
+      <c r="O3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="20">
+        <v/>
+      </c>
+      <c r="P3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="20">
+        <v/>
+      </c>
+      <c r="Q3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R3" s="20">
+        <v/>
+      </c>
+      <c r="R3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S3" s="20">
+        <v/>
+      </c>
+      <c r="S3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T3" s="21">
+        <v/>
+      </c>
+      <c r="T3" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AA3" s="3">
         <f ca="1">DATE(YEAR,$W$2,1)</f>
-        <v>43678</v>
+        <v>44044</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3. (Sat)</v>
+        <v>3. (Mon)</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -9740,7 +9741,7 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>4. (Sun)</v>
+        <v>4. (Tue)</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -9754,7 +9755,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5. (Mon)</v>
+        <v>5. (Wed)</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -9768,7 +9769,7 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6. (Tue)</v>
+        <v>6. (Thu)</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -9782,7 +9783,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7. (Wed)</v>
+        <v>7. (Fri)</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -9796,7 +9797,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>8. (Thu)</v>
+        <v>8. (Sat)</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -9810,7 +9811,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>9. (Fri)</v>
+        <v>9. (Sun)</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -9824,7 +9825,7 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10. (Sat)</v>
+        <v>10. (Mon)</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -9838,7 +9839,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>11. (Sun)</v>
+        <v>11. (Tue)</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -9852,7 +9853,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12. (Mon)</v>
+        <v>12. (Wed)</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -9866,7 +9867,7 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13. (Tue)</v>
+        <v>13. (Thu)</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -9880,7 +9881,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>14. (Wed)</v>
+        <v>14. (Fri)</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -9894,7 +9895,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15. (Thu)</v>
+        <v>15. (Sat)</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -9908,7 +9909,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16. (Fri)</v>
+        <v>16. (Sun)</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -9922,7 +9923,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17. (Sat)</v>
+        <v>17. (Mon)</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -9936,7 +9937,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18. (Sun)</v>
+        <v>18. (Tue)</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -9950,7 +9951,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19. (Mon)</v>
+        <v>19. (Wed)</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -9964,7 +9965,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20. (Tue)</v>
+        <v>20. (Thu)</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -9978,7 +9979,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>21. (Wed)</v>
+        <v>21. (Fri)</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -9992,7 +9993,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>22. (Thu)</v>
+        <v>22. (Sat)</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -10006,7 +10007,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>23. (Fri)</v>
+        <v>23. (Sun)</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -10020,7 +10021,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24. (Sat)</v>
+        <v>24. (Mon)</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -10034,7 +10035,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>25. (Sun)</v>
+        <v>25. (Tue)</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -10048,7 +10049,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26. (Mon)</v>
+        <v>26. (Wed)</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -10062,7 +10063,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>27. (Tue)</v>
+        <v>27. (Thu)</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -10076,7 +10077,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>28. (Wed)</v>
+        <v>28. (Fri)</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -10090,7 +10091,7 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>29. (Thu)</v>
+        <v>29. (Sat)</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -10104,7 +10105,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>30. (Fri)</v>
+        <v>30. (Sun)</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -10118,7 +10119,7 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>31. (Sat)</v>
+        <v>31. (Mon)</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -10176,11 +10177,11 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="87.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="88.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,4+W2,4,1,TRANS_SH))&amp;" "&amp;CHAR(10)&amp;" "&amp;YEAR</f>
         <v>September 
- 2019</v>
+ 2020</v>
       </c>
       <c r="B1" s="14" t="str">
         <f ca="1">INDIRECT(ADDRESS(LANG_ROW,27,4,1,TRANS_SH))</f>
@@ -10261,7 +10262,7 @@
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f t="shared" ref="A2:A29" ca="1" si="0">ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")"</f>
-        <v>1. (Sun)</v>
+        <v>1. (Tue)</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -10312,8 +10313,8 @@
         <v>9</v>
       </c>
       <c r="X2" s="29">
-        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),NOW()&lt;DATE(YEAR,$W$2,1)),0,MIN(NOW(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
-        <v>17.724486574072216</v>
+        <f ca="1">IF(OR(START_DATE &gt; EOMONTH(DATE(YEAR,$W$2,1),0),TODAY()&lt;DATE(YEAR,$W$2,1)),0,MIN(TODAY(),EOMONTH(DATE(YEAR,$W$2,1),0))-MAX(DATE(YEAR,$W$2,1),START_DATE)+1)</f>
+        <v>0</v>
       </c>
       <c r="AA2" s="2" t="str">
         <f ca="1">CELL("filename", A1)</f>
@@ -10323,7 +10324,7 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2. (Mon)</v>
+        <v>2. (Wed)</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -10337,47 +10338,47 @@
         <f ca="1">L2&amp;" %"</f>
         <v>Current %</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="20" t="str">
         <f ca="1">IFERROR(M$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="20">
+        <v/>
+      </c>
+      <c r="N3" s="20" t="str">
         <f t="shared" ref="N3:T3" ca="1" si="1">IFERROR(N$2/$X2*100, "")</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="20">
+        <v/>
+      </c>
+      <c r="O3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="20">
+        <v/>
+      </c>
+      <c r="P3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="20">
+        <v/>
+      </c>
+      <c r="Q3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R3" s="20">
+        <v/>
+      </c>
+      <c r="R3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S3" s="20">
+        <v/>
+      </c>
+      <c r="S3" s="20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T3" s="21">
+        <v/>
+      </c>
+      <c r="T3" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AA3" s="3">
         <f ca="1">DATE(YEAR,$W$2,1)</f>
-        <v>43709</v>
+        <v>44075</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3. (Tue)</v>
+        <v>3. (Thu)</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -10431,7 +10432,7 @@
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>4. (Wed)</v>
+        <v>4. (Fri)</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -10445,7 +10446,7 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5. (Thu)</v>
+        <v>5. (Sat)</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -10459,7 +10460,7 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6. (Fri)</v>
+        <v>6. (Sun)</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -10473,7 +10474,7 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7. (Sat)</v>
+        <v>7. (Mon)</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -10487,7 +10488,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>8. (Sun)</v>
+        <v>8. (Tue)</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -10501,7 +10502,7 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>9. (Mon)</v>
+        <v>9. (Wed)</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -10515,7 +10516,7 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>10. (Tue)</v>
+        <v>10. (Thu)</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -10529,7 +10530,7 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>11. (Wed)</v>
+        <v>11. (Fri)</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -10543,7 +10544,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12. (Thu)</v>
+        <v>12. (Sat)</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -10557,7 +10558,7 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13. (Fri)</v>
+        <v>13. (Sun)</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -10571,7 +10572,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>14. (Sat)</v>
+        <v>14. (Mon)</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -10585,7 +10586,7 @@
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15. (Sun)</v>
+        <v>15. (Tue)</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -10599,7 +10600,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16. (Mon)</v>
+        <v>16. (Wed)</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -10613,7 +10614,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17. (Tue)</v>
+        <v>17. (Thu)</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -10627,7 +10628,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18. (Wed)</v>
+        <v>18. (Fri)</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -10641,7 +10642,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>19. (Thu)</v>
+        <v>19. (Sat)</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -10655,7 +10656,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20. (Fri)</v>
+        <v>20. (Sun)</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -10669,7 +10670,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>21. (Sat)</v>
+        <v>21. (Mon)</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -10683,7 +10684,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>22. (Sun)</v>
+        <v>22. (Tue)</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -10697,7 +10698,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>23. (Mon)</v>
+        <v>23. (Wed)</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -10711,7 +10712,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>24. (Tue)</v>
+        <v>24. (Thu)</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -10725,7 +10726,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>25. (Wed)</v>
+        <v>25. (Fri)</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -10739,7 +10740,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>26. (Thu)</v>
+        <v>26. (Sat)</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -10753,7 +10754,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>27. (Fri)</v>
+        <v>27. (Sun)</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -10767,7 +10768,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>28. (Sat)</v>
+        <v>28. (Mon)</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -10781,7 +10782,7 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>29. (Sun)</v>
+        <v>29. (Tue)</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -10795,7 +10796,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="str">
         <f ca="1">IF(ROW()-1 &gt; $AA$4,"",ROW()-1&amp;". ("&amp;INDIRECT(ADDRESS(LANG_ROW,17+WEEKDAY(DATE(YEAR,$W$2,ROW()-1),2),4,1,TRANS_SH))&amp;")")</f>
-        <v>30. (Mon)</v>
+        <v>30. (Wed)</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>

</xml_diff>